<commit_message>
there will be at this moment 4 new mod setups
</commit_message>
<xml_diff>
--- a/mode/AllUnlocked/NewEngineFormulas.xlsx
+++ b/mode/AllUnlocked/NewEngineFormulas.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -470,7 +469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -543,35 +542,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -584,8 +559,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -893,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,10 +898,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -949,11 +922,11 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="5">
         <f>MIN(F20:F164)</f>
-        <v>310</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D4" s="5">
         <f>MAX(F20:F164)</f>
-        <v>2400</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,7 +973,7 @@
         <v>340</v>
       </c>
       <c r="D8" s="11">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E8" s="5">
         <f>IF($D$6&lt;=$C$8,1,0)*$D$8+0+0+0+0+0+0+0+0+0</f>
@@ -1015,8 +988,8 @@
       <c r="C9" s="5">
         <v>360</v>
       </c>
-      <c r="D9" s="12">
-        <v>1.2</v>
+      <c r="D9" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E9" s="5">
         <f>IF(AND($D$6&gt;$C$8,$D$6&lt;=$C$9),1,0)*$D$9</f>
@@ -1031,8 +1004,8 @@
       <c r="C10" s="5">
         <v>400</v>
       </c>
-      <c r="D10" s="12">
-        <v>1.4</v>
+      <c r="D10" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E10" s="5">
         <f>IF(AND($D$6&gt;$C$9,$D$6&lt;=$C$10),1,0)*$D$10</f>
@@ -1047,8 +1020,8 @@
       <c r="C11" s="5">
         <v>425</v>
       </c>
-      <c r="D11" s="12">
-        <v>1.6</v>
+      <c r="D11" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E11" s="5">
         <f>IF(AND($D$6&gt;$C$10,$D$6&lt;=$C$11),1,0)*$D$11</f>
@@ -1063,8 +1036,8 @@
       <c r="C12" s="5">
         <v>450</v>
       </c>
-      <c r="D12" s="12">
-        <v>2</v>
+      <c r="D12" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E12" s="5">
         <f>IF(AND($D$6&gt;$C$11,$D$6&lt;=$C$12),1,0)*$D$12</f>
@@ -1079,8 +1052,8 @@
       <c r="C13" s="5">
         <v>475</v>
       </c>
-      <c r="D13" s="12">
-        <v>2.4</v>
+      <c r="D13" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E13" s="5">
         <f>IF(AND($D$6&gt;$C$12,$D$6&lt;=$C$13),1,0)*$D$13</f>
@@ -1095,8 +1068,8 @@
       <c r="C14" s="5">
         <v>500</v>
       </c>
-      <c r="D14" s="12">
-        <v>2.6</v>
+      <c r="D14" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E14" s="5">
         <f>IF(AND($D$6&gt;$C$13,$D$6&lt;=$C$14),1,0)*$D$14</f>
@@ -1111,12 +1084,12 @@
       <c r="C15" s="5">
         <v>550</v>
       </c>
-      <c r="D15" s="12">
-        <v>2.8</v>
+      <c r="D15" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E15" s="5">
         <f>IF(AND($D$6&gt;$C$14,$D$6&lt;=$C$15),1,0)*$D$15</f>
-        <v>2.8</v>
+        <v>1E-4</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1127,8 +1100,8 @@
       <c r="C16" s="5">
         <v>600</v>
       </c>
-      <c r="D16" s="12">
-        <v>3</v>
+      <c r="D16" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E16" s="5">
         <f>IF(AND($D$6&gt;$C$15,$D$6&lt;=$C$16),1,0)*$D$16</f>
@@ -1143,8 +1116,8 @@
       <c r="C17" s="5">
         <v>750</v>
       </c>
-      <c r="D17" s="13">
-        <v>3.2</v>
+      <c r="D17" s="11">
+        <v>1E-4</v>
       </c>
       <c r="E17" s="5">
         <f>IF(AND($D$6&gt;$C$16,$D$6&lt;=$C$17),1,0)*$D$17</f>
@@ -1153,29 +1126,29 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1194,7 +1167,7 @@
         <f>($F$2*C19)+($H$2*D19)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="16"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1205,14 +1178,14 @@
       </c>
       <c r="F20" s="1">
         <f>($E$19+B20)*(IF(B20&lt;=$C$8,1,0)*$D$8+IF(AND(B20&gt;$C$8,B20&lt;=$C$9),1,0)*$D$9+IF(AND(B20&gt;$C$9,B20&lt;=$C$10),1,0)*$D$10+IF(AND(B20&gt;$C$10,B20&lt;=$C$11),1,0)*$D$11+IF(AND(B20&gt;$C$11,B20&lt;=$C$12),1,0)*$D$12+IF(AND(B20&gt;$C$12,B20&lt;=$C$13),1,0)*$D$13+IF(AND(B20&gt;$C$13,B20&lt;=$C$14),1,0)*$D$14+IF(AND(B20&gt;$C$14,B20&lt;=$C$15),1,0)*$D$15+IF(AND(B20&gt;$C$15,B20&lt;=$C$16),1,0)*$D$16+IF(AND(B20&gt;$C$16,B20&lt;=$C$17),1,0)*$D$17)</f>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="14">
         <f>ROUND(((F20-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1224,14 +1197,14 @@
       </c>
       <c r="F21" s="1">
         <f>($E$19+B21)*(IF(B21&lt;=$C$8,1,0)*$D$8+IF(AND(B21&gt;$C$8,B21&lt;=$C$9),1,0)*$D$9+IF(AND(B21&gt;$C$9,B21&lt;=$C$10),1,0)*$D$10+IF(AND(B21&gt;$C$10,B21&lt;=$C$11),1,0)*$D$11+IF(AND(B21&gt;$C$11,B21&lt;=$C$12),1,0)*$D$12+IF(AND(B21&gt;$C$12,B21&lt;=$C$13),1,0)*$D$13+IF(AND(B21&gt;$C$13,B21&lt;=$C$14),1,0)*$D$14+IF(AND(B21&gt;$C$14,B21&lt;=$C$15),1,0)*$D$15+IF(AND(B21&gt;$C$15,B21&lt;=$C$16),1,0)*$D$16+IF(AND(B21&gt;$C$16,B21&lt;=$C$17),1,0)*$D$17)</f>
-        <v>656</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G21" s="1">
         <v>6</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="14">
         <f>ROUND(((F21-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1243,14 +1216,14 @@
       </c>
       <c r="F22" s="1">
         <f>($E$19+B22)*(IF(B22&lt;=$C$8,1,0)*$D$8+IF(AND(B22&gt;$C$8,B22&lt;=$C$9),1,0)*$D$9+IF(AND(B22&gt;$C$9,B22&lt;=$C$10),1,0)*$D$10+IF(AND(B22&gt;$C$10,B22&lt;=$C$11),1,0)*$D$11+IF(AND(B22&gt;$C$11,B22&lt;=$C$12),1,0)*$D$12+IF(AND(B22&gt;$C$12,B22&lt;=$C$13),1,0)*$D$13+IF(AND(B22&gt;$C$13,B22&lt;=$C$14),1,0)*$D$14+IF(AND(B22&gt;$C$14,B22&lt;=$C$15),1,0)*$D$15+IF(AND(B22&gt;$C$15,B22&lt;=$C$16),1,0)*$D$16+IF(AND(B22&gt;$C$16,B22&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G22" s="1">
         <v>10</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="14">
         <f>ROUND(((F22-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1262,14 +1235,14 @@
       </c>
       <c r="F23" s="1">
         <f>($E$19+B23)*(IF(B23&lt;=$C$8,1,0)*$D$8+IF(AND(B23&gt;$C$8,B23&lt;=$C$9),1,0)*$D$9+IF(AND(B23&gt;$C$9,B23&lt;=$C$10),1,0)*$D$10+IF(AND(B23&gt;$C$10,B23&lt;=$C$11),1,0)*$D$11+IF(AND(B23&gt;$C$11,B23&lt;=$C$12),1,0)*$D$12+IF(AND(B23&gt;$C$12,B23&lt;=$C$13),1,0)*$D$13+IF(AND(B23&gt;$C$13,B23&lt;=$C$14),1,0)*$D$14+IF(AND(B23&gt;$C$14,B23&lt;=$C$15),1,0)*$D$15+IF(AND(B23&gt;$C$15,B23&lt;=$C$16),1,0)*$D$16+IF(AND(B23&gt;$C$16,B23&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1428</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="G23" s="1">
         <v>16</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="14">
         <f>ROUND(((F23-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1287,7 +1260,7 @@
         <f>($F$2*C24)+($H$2*D24)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="16"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1298,14 +1271,14 @@
       </c>
       <c r="F25" s="1">
         <f>($E$24+B25)*(IF(B25&lt;=$C$8,1,0)*$D$8+IF(AND(B25&gt;$C$8,B25&lt;=$C$9),1,0)*$D$9+IF(AND(B25&gt;$C$9,B25&lt;=$C$10),1,0)*$D$10+IF(AND(B25&gt;$C$10,B25&lt;=$C$11),1,0)*$D$11+IF(AND(B25&gt;$C$11,B25&lt;=$C$12),1,0)*$D$12+IF(AND(B25&gt;$C$12,B25&lt;=$C$13),1,0)*$D$13+IF(AND(B25&gt;$C$13,B25&lt;=$C$14),1,0)*$D$14+IF(AND(B25&gt;$C$14,B25&lt;=$C$15),1,0)*$D$15+IF(AND(B25&gt;$C$15,B25&lt;=$C$16),1,0)*$D$16+IF(AND(B25&gt;$C$16,B25&lt;=$C$17),1,0)*$D$17)</f>
-        <v>518</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="14">
         <f t="shared" ref="H25:H32" si="0">ROUND(((F25-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1317,14 +1290,14 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" ref="F26:F32" si="1">($E$24+B26)*(IF(B26&lt;=$C$8,1,0)*$D$8+IF(AND(B26&gt;$C$8,B26&lt;=$C$9),1,0)*$D$9+IF(AND(B26&gt;$C$9,B26&lt;=$C$10),1,0)*$D$10+IF(AND(B26&gt;$C$10,B26&lt;=$C$11),1,0)*$D$11+IF(AND(B26&gt;$C$11,B26&lt;=$C$12),1,0)*$D$12+IF(AND(B26&gt;$C$12,B26&lt;=$C$13),1,0)*$D$13+IF(AND(B26&gt;$C$13,B26&lt;=$C$14),1,0)*$D$14+IF(AND(B26&gt;$C$14,B26&lt;=$C$15),1,0)*$D$15+IF(AND(B26&gt;$C$15,B26&lt;=$C$16),1,0)*$D$16+IF(AND(B26&gt;$C$16,B26&lt;=$C$17),1,0)*$D$17)</f>
-        <v>656</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1336,14 +1309,14 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="1"/>
-        <v>870</v>
+        <v>4.3500000000000004E-2</v>
       </c>
       <c r="G27" s="1">
         <v>6</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1355,14 +1328,14 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="G28" s="1">
         <v>8</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1374,14 +1347,14 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G29" s="1">
         <v>10</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="14">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1393,14 +1366,14 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G30" s="1">
         <v>14</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="14">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1412,14 +1385,14 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
-        <v>1428</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="G31" s="1">
         <v>16</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="14">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1431,14 +1404,14 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
-        <v>1484</v>
+        <v>5.3000000000000005E-2</v>
       </c>
       <c r="G32" s="1">
         <v>18</v>
       </c>
-      <c r="H32" s="16">
+      <c r="H32" s="14">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1456,7 +1429,7 @@
         <f>($F$2*C33)+($H$2*D33)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="16"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1467,14 +1440,14 @@
       </c>
       <c r="F34" s="1">
         <f>($E$33+B34)*(IF(B34&lt;=$C$8,1,0)*$D$8+IF(AND(B34&gt;$C$8,B34&lt;=$C$9),1,0)*$D$9+IF(AND(B34&gt;$C$9,B34&lt;=$C$10),1,0)*$D$10+IF(AND(B34&gt;$C$10,B34&lt;=$C$11),1,0)*$D$11+IF(AND(B34&gt;$C$11,B34&lt;=$C$12),1,0)*$D$12+IF(AND(B34&gt;$C$12,B34&lt;=$C$13),1,0)*$D$13+IF(AND(B34&gt;$C$13,B34&lt;=$C$14),1,0)*$D$14+IF(AND(B34&gt;$C$14,B34&lt;=$C$15),1,0)*$D$15+IF(AND(B34&gt;$C$15,B34&lt;=$C$16),1,0)*$D$16+IF(AND(B34&gt;$C$16,B34&lt;=$C$17),1,0)*$D$17)</f>
-        <v>310</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="14">
         <f t="shared" ref="H34:H41" si="2">ROUND(((F34-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1486,14 +1459,14 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ref="F35:F41" si="3">($E$33+B35)*(IF(B35&lt;=$C$8,1,0)*$D$8+IF(AND(B35&gt;$C$8,B35&lt;=$C$9),1,0)*$D$9+IF(AND(B35&gt;$C$9,B35&lt;=$C$10),1,0)*$D$10+IF(AND(B35&gt;$C$10,B35&lt;=$C$11),1,0)*$D$11+IF(AND(B35&gt;$C$11,B35&lt;=$C$12),1,0)*$D$12+IF(AND(B35&gt;$C$12,B35&lt;=$C$13),1,0)*$D$13+IF(AND(B35&gt;$C$13,B35&lt;=$C$14),1,0)*$D$14+IF(AND(B35&gt;$C$14,B35&lt;=$C$15),1,0)*$D$15+IF(AND(B35&gt;$C$15,B35&lt;=$C$16),1,0)*$D$16+IF(AND(B35&gt;$C$16,B35&lt;=$C$17),1,0)*$D$17)</f>
-        <v>330</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G35" s="1">
         <v>6</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35" s="14">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1505,14 +1478,14 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" si="3"/>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G36" s="1">
         <v>8</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36" s="14">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1524,14 +1497,14 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" si="3"/>
-        <v>560</v>
+        <v>0.04</v>
       </c>
       <c r="G37" s="1">
         <v>9</v>
       </c>
-      <c r="H37" s="16">
+      <c r="H37" s="14">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1543,14 +1516,14 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" si="3"/>
-        <v>672</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G38" s="1">
         <v>10</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38" s="14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1562,14 +1535,14 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="3"/>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G39" s="1">
         <v>12</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="14">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1581,14 +1554,14 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" si="3"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G40" s="1">
         <v>14</v>
       </c>
-      <c r="H40" s="16">
+      <c r="H40" s="14">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1600,14 +1573,14 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" si="3"/>
-        <v>1680</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="G41" s="1">
         <v>16</v>
       </c>
-      <c r="H41" s="16">
+      <c r="H41" s="14">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1625,7 +1598,7 @@
         <f>($F$2*C42)+($H$2*D42)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="16"/>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1636,14 +1609,14 @@
       </c>
       <c r="F43" s="1">
         <f>($E$42+B43)*(IF(B43&lt;=$C$8,1,0)*$D$8+IF(AND(B43&gt;$C$8,B43&lt;=$C$9),1,0)*$D$9+IF(AND(B43&gt;$C$9,B43&lt;=$C$10),1,0)*$D$10+IF(AND(B43&gt;$C$10,B43&lt;=$C$11),1,0)*$D$11+IF(AND(B43&gt;$C$11,B43&lt;=$C$12),1,0)*$D$12+IF(AND(B43&gt;$C$12,B43&lt;=$C$13),1,0)*$D$13+IF(AND(B43&gt;$C$13,B43&lt;=$C$14),1,0)*$D$14+IF(AND(B43&gt;$C$14,B43&lt;=$C$15),1,0)*$D$15+IF(AND(B43&gt;$C$15,B43&lt;=$C$16),1,0)*$D$16+IF(AND(B43&gt;$C$16,B43&lt;=$C$17),1,0)*$D$17)</f>
-        <v>310</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
       </c>
-      <c r="H43" s="16">
+      <c r="H43" s="14">
         <f t="shared" ref="H43:H49" si="4">ROUND(((F43-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1655,14 +1628,14 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" ref="F44:F49" si="5">($E$42+B44)*(IF(B44&lt;=$C$8,1,0)*$D$8+IF(AND(B44&gt;$C$8,B44&lt;=$C$9),1,0)*$D$9+IF(AND(B44&gt;$C$9,B44&lt;=$C$10),1,0)*$D$10+IF(AND(B44&gt;$C$10,B44&lt;=$C$11),1,0)*$D$11+IF(AND(B44&gt;$C$11,B44&lt;=$C$12),1,0)*$D$12+IF(AND(B44&gt;$C$12,B44&lt;=$C$13),1,0)*$D$13+IF(AND(B44&gt;$C$13,B44&lt;=$C$14),1,0)*$D$14+IF(AND(B44&gt;$C$14,B44&lt;=$C$15),1,0)*$D$15+IF(AND(B44&gt;$C$15,B44&lt;=$C$16),1,0)*$D$16+IF(AND(B44&gt;$C$16,B44&lt;=$C$17),1,0)*$D$17)</f>
-        <v>330</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G44" s="1">
         <v>6</v>
       </c>
-      <c r="H44" s="16">
+      <c r="H44" s="14">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1674,14 +1647,14 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" si="5"/>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G45" s="1">
         <v>8</v>
       </c>
-      <c r="H45" s="16">
+      <c r="H45" s="14">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1693,14 +1666,14 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" si="5"/>
-        <v>672</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G46" s="1">
         <v>10</v>
       </c>
-      <c r="H46" s="16">
+      <c r="H46" s="14">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1712,14 +1685,14 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" si="5"/>
-        <v>900</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="G47" s="1">
         <v>12</v>
       </c>
-      <c r="H47" s="16">
+      <c r="H47" s="14">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1731,14 +1704,14 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" si="5"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G48" s="1">
         <v>14</v>
       </c>
-      <c r="H48" s="16">
+      <c r="H48" s="14">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1750,14 +1723,14 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" si="5"/>
-        <v>1680</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="G49" s="1">
         <v>16</v>
       </c>
-      <c r="H49" s="16">
+      <c r="H49" s="14">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1775,7 +1748,7 @@
         <f>($F$2*C50)+($H$2*D50)</f>
         <v>0</v>
       </c>
-      <c r="H50" s="16"/>
+      <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -1786,14 +1759,14 @@
       </c>
       <c r="F51" s="1">
         <f>($E$50+B51)*(IF(B51&lt;=$C$8,1,0)*$D$8+IF(AND(B51&gt;$C$8,B51&lt;=$C$9),1,0)*$D$9+IF(AND(B51&gt;$C$9,B51&lt;=$C$10),1,0)*$D$10+IF(AND(B51&gt;$C$10,B51&lt;=$C$11),1,0)*$D$11+IF(AND(B51&gt;$C$11,B51&lt;=$C$12),1,0)*$D$12+IF(AND(B51&gt;$C$12,B51&lt;=$C$13),1,0)*$D$13+IF(AND(B51&gt;$C$13,B51&lt;=$C$14),1,0)*$D$14+IF(AND(B51&gt;$C$14,B51&lt;=$C$15),1,0)*$D$15+IF(AND(B51&gt;$C$15,B51&lt;=$C$16),1,0)*$D$16+IF(AND(B51&gt;$C$16,B51&lt;=$C$17),1,0)*$D$17)</f>
-        <v>320</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
       </c>
-      <c r="H51" s="16">
+      <c r="H51" s="14">
         <f t="shared" ref="H51:H57" si="6">ROUND(((F51-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1805,14 +1778,14 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" ref="F52:F57" si="7">($E$50+B52)*(IF(B52&lt;=$C$8,1,0)*$D$8+IF(AND(B52&gt;$C$8,B52&lt;=$C$9),1,0)*$D$9+IF(AND(B52&gt;$C$9,B52&lt;=$C$10),1,0)*$D$10+IF(AND(B52&gt;$C$10,B52&lt;=$C$11),1,0)*$D$11+IF(AND(B52&gt;$C$11,B52&lt;=$C$12),1,0)*$D$12+IF(AND(B52&gt;$C$12,B52&lt;=$C$13),1,0)*$D$13+IF(AND(B52&gt;$C$13,B52&lt;=$C$14),1,0)*$D$14+IF(AND(B52&gt;$C$14,B52&lt;=$C$15),1,0)*$D$15+IF(AND(B52&gt;$C$15,B52&lt;=$C$16),1,0)*$D$16+IF(AND(B52&gt;$C$16,B52&lt;=$C$17),1,0)*$D$17)</f>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G52" s="1">
         <v>6</v>
       </c>
-      <c r="H52" s="16">
+      <c r="H52" s="14">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1824,14 +1797,14 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
-        <v>560</v>
+        <v>0.04</v>
       </c>
       <c r="G53" s="1">
         <v>8</v>
       </c>
-      <c r="H53" s="16">
+      <c r="H53" s="14">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1843,14 +1816,14 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G54" s="1">
         <v>10</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H54" s="14">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1862,14 +1835,14 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" si="7"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G55" s="1">
         <v>12</v>
       </c>
-      <c r="H55" s="16">
+      <c r="H55" s="14">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1881,14 +1854,14 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" si="7"/>
-        <v>1512</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G56" s="1">
         <v>14</v>
       </c>
-      <c r="H56" s="16">
+      <c r="H56" s="14">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1900,14 +1873,14 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" si="7"/>
-        <v>2176</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="G57" s="1">
         <v>16</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="14">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1925,7 +1898,7 @@
         <f>($F$2*C58)+($H$2*D58)</f>
         <v>0</v>
       </c>
-      <c r="H58" s="16"/>
+      <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -1936,14 +1909,14 @@
       </c>
       <c r="F59" s="1">
         <f>($E$58+B59)*(IF(B59&lt;=$C$8,1,0)*$D$8+IF(AND(B59&gt;$C$8,B59&lt;=$C$9),1,0)*$D$9+IF(AND(B59&gt;$C$9,B59&lt;=$C$10),1,0)*$D$10+IF(AND(B59&gt;$C$10,B59&lt;=$C$11),1,0)*$D$11+IF(AND(B59&gt;$C$11,B59&lt;=$C$12),1,0)*$D$12+IF(AND(B59&gt;$C$12,B59&lt;=$C$13),1,0)*$D$13+IF(AND(B59&gt;$C$13,B59&lt;=$C$14),1,0)*$D$14+IF(AND(B59&gt;$C$14,B59&lt;=$C$15),1,0)*$D$15+IF(AND(B59&gt;$C$15,B59&lt;=$C$16),1,0)*$D$16+IF(AND(B59&gt;$C$16,B59&lt;=$C$17),1,0)*$D$17)</f>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
       </c>
-      <c r="H59" s="16">
+      <c r="H59" s="14">
         <f t="shared" ref="H59:H65" si="8">ROUND(((F59-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1955,14 +1928,14 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" ref="F60:F65" si="9">($E$58+B60)*(IF(B60&lt;=$C$8,1,0)*$D$8+IF(AND(B60&gt;$C$8,B60&lt;=$C$9),1,0)*$D$9+IF(AND(B60&gt;$C$9,B60&lt;=$C$10),1,0)*$D$10+IF(AND(B60&gt;$C$10,B60&lt;=$C$11),1,0)*$D$11+IF(AND(B60&gt;$C$11,B60&lt;=$C$12),1,0)*$D$12+IF(AND(B60&gt;$C$12,B60&lt;=$C$13),1,0)*$D$13+IF(AND(B60&gt;$C$13,B60&lt;=$C$14),1,0)*$D$14+IF(AND(B60&gt;$C$14,B60&lt;=$C$15),1,0)*$D$15+IF(AND(B60&gt;$C$15,B60&lt;=$C$16),1,0)*$D$16+IF(AND(B60&gt;$C$16,B60&lt;=$C$17),1,0)*$D$17)</f>
-        <v>560</v>
+        <v>0.04</v>
       </c>
       <c r="G60" s="1">
         <v>6</v>
       </c>
-      <c r="H60" s="16">
+      <c r="H60" s="14">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1974,14 +1947,14 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" si="9"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G61" s="1">
         <v>8</v>
       </c>
-      <c r="H61" s="16">
+      <c r="H61" s="14">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1993,14 +1966,14 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" si="9"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G62" s="1">
         <v>12</v>
       </c>
-      <c r="H62" s="16">
+      <c r="H62" s="14">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2012,14 +1985,14 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" si="9"/>
-        <v>1456</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="G63" s="1">
         <v>16</v>
       </c>
-      <c r="H63" s="16">
+      <c r="H63" s="14">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2031,14 +2004,14 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" si="9"/>
-        <v>1680</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="G64" s="1">
         <v>18</v>
       </c>
-      <c r="H64" s="16">
+      <c r="H64" s="14">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2050,14 +2023,14 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" si="9"/>
-        <v>2048</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G65" s="1">
         <v>20</v>
       </c>
-      <c r="H65" s="16">
+      <c r="H65" s="14">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2075,7 +2048,7 @@
         <f>($F$2*C66)+($H$2*D66)</f>
         <v>0</v>
       </c>
-      <c r="H66" s="16"/>
+      <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -2086,14 +2059,14 @@
       </c>
       <c r="F67" s="1">
         <f>($E$66+B67)*(IF(B67&lt;=$C$8,1,0)*$D$8+IF(AND(B67&gt;$C$8,B67&lt;=$C$9),1,0)*$D$9+IF(AND(B67&gt;$C$9,B67&lt;=$C$10),1,0)*$D$10+IF(AND(B67&gt;$C$10,B67&lt;=$C$11),1,0)*$D$11+IF(AND(B67&gt;$C$11,B67&lt;=$C$12),1,0)*$D$12+IF(AND(B67&gt;$C$12,B67&lt;=$C$13),1,0)*$D$13+IF(AND(B67&gt;$C$13,B67&lt;=$C$14),1,0)*$D$14+IF(AND(B67&gt;$C$14,B67&lt;=$C$15),1,0)*$D$15+IF(AND(B67&gt;$C$15,B67&lt;=$C$16),1,0)*$D$16+IF(AND(B67&gt;$C$16,B67&lt;=$C$17),1,0)*$D$17)</f>
-        <v>320</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
       </c>
-      <c r="H67" s="16">
+      <c r="H67" s="14">
         <f t="shared" ref="H67:H75" si="10">ROUND(((F67-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2105,14 +2078,14 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" ref="F68:F75" si="11">($E$66+B68)*(IF(B68&lt;=$C$8,1,0)*$D$8+IF(AND(B68&gt;$C$8,B68&lt;=$C$9),1,0)*$D$9+IF(AND(B68&gt;$C$9,B68&lt;=$C$10),1,0)*$D$10+IF(AND(B68&gt;$C$10,B68&lt;=$C$11),1,0)*$D$11+IF(AND(B68&gt;$C$11,B68&lt;=$C$12),1,0)*$D$12+IF(AND(B68&gt;$C$12,B68&lt;=$C$13),1,0)*$D$13+IF(AND(B68&gt;$C$13,B68&lt;=$C$14),1,0)*$D$14+IF(AND(B68&gt;$C$14,B68&lt;=$C$15),1,0)*$D$15+IF(AND(B68&gt;$C$15,B68&lt;=$C$16),1,0)*$D$16+IF(AND(B68&gt;$C$16,B68&lt;=$C$17),1,0)*$D$17)</f>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G68" s="1">
         <v>6</v>
       </c>
-      <c r="H68" s="16">
+      <c r="H68" s="14">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2124,14 +2097,14 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" si="11"/>
-        <v>652.80000000000007</v>
+        <v>4.0800000000000003E-2</v>
       </c>
       <c r="G69" s="1">
         <v>8</v>
       </c>
-      <c r="H69" s="16">
+      <c r="H69" s="14">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2143,14 +2116,14 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="11"/>
-        <v>870</v>
+        <v>4.3500000000000004E-2</v>
       </c>
       <c r="G70" s="1">
         <v>10</v>
       </c>
-      <c r="H70" s="16">
+      <c r="H70" s="14">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2162,14 +2135,14 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" si="11"/>
-        <v>1094.3999999999999</v>
+        <v>4.5600000000000002E-2</v>
       </c>
       <c r="G71" s="1">
         <v>12</v>
       </c>
-      <c r="H71" s="16">
+      <c r="H71" s="14">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2181,14 +2154,14 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" si="11"/>
-        <v>1237.6000000000001</v>
+        <v>4.7600000000000003E-2</v>
       </c>
       <c r="G72" s="1">
         <v>14</v>
       </c>
-      <c r="H72" s="16">
+      <c r="H72" s="14">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2200,14 +2173,14 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" si="11"/>
-        <v>1428</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="G73" s="1">
         <v>16</v>
       </c>
-      <c r="H73" s="16">
+      <c r="H73" s="14">
         <f t="shared" si="10"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2219,14 +2192,14 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" si="11"/>
-        <v>1653</v>
+        <v>5.5100000000000003E-2</v>
       </c>
       <c r="G74" s="1">
         <v>18</v>
       </c>
-      <c r="H74" s="16">
+      <c r="H74" s="14">
         <f t="shared" si="10"/>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2238,14 +2211,14 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" si="11"/>
-        <v>1794</v>
+        <v>5.9800000000000006E-2</v>
       </c>
       <c r="G75" s="1">
         <v>20</v>
       </c>
-      <c r="H75" s="16">
+      <c r="H75" s="14">
         <f t="shared" si="10"/>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2263,7 +2236,7 @@
         <f>($F$2*C76)+($H$2*D76)</f>
         <v>0</v>
       </c>
-      <c r="H76" s="16"/>
+      <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -2274,14 +2247,14 @@
       </c>
       <c r="F77" s="1">
         <f>($E$76+B77)*(IF(B77&lt;=$C$8,1,0)*$D$8+IF(AND(B77&gt;$C$8,B77&lt;=$C$9),1,0)*$D$9+IF(AND(B77&gt;$C$9,B77&lt;=$C$10),1,0)*$D$10+IF(AND(B77&gt;$C$10,B77&lt;=$C$11),1,0)*$D$11+IF(AND(B77&gt;$C$11,B77&lt;=$C$12),1,0)*$D$12+IF(AND(B77&gt;$C$12,B77&lt;=$C$13),1,0)*$D$13+IF(AND(B77&gt;$C$13,B77&lt;=$C$14),1,0)*$D$14+IF(AND(B77&gt;$C$14,B77&lt;=$C$15),1,0)*$D$15+IF(AND(B77&gt;$C$15,B77&lt;=$C$16),1,0)*$D$16+IF(AND(B77&gt;$C$16,B77&lt;=$C$17),1,0)*$D$17)</f>
-        <v>673.6</v>
+        <v>4.2100000000000005E-2</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
       </c>
-      <c r="H77" s="16">
+      <c r="H77" s="14">
         <f t="shared" ref="H77:H83" si="12">ROUND(((F77-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2293,14 +2266,14 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" ref="F78:F83" si="13">($E$76+B78)*(IF(B78&lt;=$C$8,1,0)*$D$8+IF(AND(B78&gt;$C$8,B78&lt;=$C$9),1,0)*$D$9+IF(AND(B78&gt;$C$9,B78&lt;=$C$10),1,0)*$D$10+IF(AND(B78&gt;$C$10,B78&lt;=$C$11),1,0)*$D$11+IF(AND(B78&gt;$C$11,B78&lt;=$C$12),1,0)*$D$12+IF(AND(B78&gt;$C$12,B78&lt;=$C$13),1,0)*$D$13+IF(AND(B78&gt;$C$13,B78&lt;=$C$14),1,0)*$D$14+IF(AND(B78&gt;$C$14,B78&lt;=$C$15),1,0)*$D$15+IF(AND(B78&gt;$C$15,B78&lt;=$C$16),1,0)*$D$16+IF(AND(B78&gt;$C$16,B78&lt;=$C$17),1,0)*$D$17)</f>
-        <v>898</v>
+        <v>4.4900000000000002E-2</v>
       </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
-      <c r="H78" s="16">
+      <c r="H78" s="14">
         <f t="shared" si="12"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2312,14 +2285,14 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" si="13"/>
-        <v>1237.6000000000001</v>
+        <v>4.7600000000000003E-2</v>
       </c>
       <c r="G79" s="1">
         <v>10</v>
       </c>
-      <c r="H79" s="16">
+      <c r="H79" s="14">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2331,14 +2304,14 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" si="13"/>
-        <v>1428</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="G80" s="1">
         <v>12</v>
       </c>
-      <c r="H80" s="16">
+      <c r="H80" s="14">
         <f t="shared" si="12"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2350,14 +2323,14 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" si="13"/>
-        <v>1447.6</v>
+        <v>5.1700000000000003E-2</v>
       </c>
       <c r="G81" s="1">
         <v>14</v>
       </c>
-      <c r="H81" s="16">
+      <c r="H81" s="14">
         <f t="shared" si="12"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2369,14 +2342,14 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" si="13"/>
-        <v>1734</v>
+        <v>5.7800000000000004E-2</v>
       </c>
       <c r="G82" s="1">
         <v>16</v>
       </c>
-      <c r="H82" s="16">
+      <c r="H82" s="14">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2388,14 +2361,14 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" si="13"/>
-        <v>2000</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G83" s="1">
         <v>20</v>
       </c>
-      <c r="H83" s="16">
+      <c r="H83" s="14">
         <f t="shared" si="12"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -2413,7 +2386,7 @@
         <f>($F$2*C84)+($H$2*D84)</f>
         <v>0</v>
       </c>
-      <c r="H84" s="16"/>
+      <c r="H84" s="14"/>
     </row>
     <row r="85" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
@@ -2424,14 +2397,14 @@
       </c>
       <c r="F85" s="1">
         <f>($E$84+B85)*(IF(B85&lt;=$C$8,1,0)*$D$8+IF(AND(B85&gt;$C$8,B85&lt;=$C$9),1,0)*$D$9+IF(AND(B85&gt;$C$9,B85&lt;=$C$10),1,0)*$D$10+IF(AND(B85&gt;$C$10,B85&lt;=$C$11),1,0)*$D$11+IF(AND(B85&gt;$C$11,B85&lt;=$C$12),1,0)*$D$12+IF(AND(B85&gt;$C$12,B85&lt;=$C$13),1,0)*$D$13+IF(AND(B85&gt;$C$13,B85&lt;=$C$14),1,0)*$D$14+IF(AND(B85&gt;$C$14,B85&lt;=$C$15),1,0)*$D$15+IF(AND(B85&gt;$C$15,B85&lt;=$C$16),1,0)*$D$16+IF(AND(B85&gt;$C$16,B85&lt;=$C$17),1,0)*$D$17)</f>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
       </c>
-      <c r="H85" s="16">
+      <c r="H85" s="14">
         <f>ROUND(((F85-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2443,14 +2416,14 @@
       </c>
       <c r="F86" s="1">
         <f>($E$84+B86)*(IF(B86&lt;=$C$8,1,0)*$D$8+IF(AND(B86&gt;$C$8,B86&lt;=$C$9),1,0)*$D$9+IF(AND(B86&gt;$C$9,B86&lt;=$C$10),1,0)*$D$10+IF(AND(B86&gt;$C$10,B86&lt;=$C$11),1,0)*$D$11+IF(AND(B86&gt;$C$11,B86&lt;=$C$12),1,0)*$D$12+IF(AND(B86&gt;$C$12,B86&lt;=$C$13),1,0)*$D$13+IF(AND(B86&gt;$C$13,B86&lt;=$C$14),1,0)*$D$14+IF(AND(B86&gt;$C$14,B86&lt;=$C$15),1,0)*$D$15+IF(AND(B86&gt;$C$15,B86&lt;=$C$16),1,0)*$D$16+IF(AND(B86&gt;$C$16,B86&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G86" s="1">
         <v>10</v>
       </c>
-      <c r="H86" s="16">
+      <c r="H86" s="14">
         <f>ROUND(((F86-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2462,14 +2435,14 @@
       </c>
       <c r="F87" s="1">
         <f>($E$84+B87)*(IF(B87&lt;=$C$8,1,0)*$D$8+IF(AND(B87&gt;$C$8,B87&lt;=$C$9),1,0)*$D$9+IF(AND(B87&gt;$C$9,B87&lt;=$C$10),1,0)*$D$10+IF(AND(B87&gt;$C$10,B87&lt;=$C$11),1,0)*$D$11+IF(AND(B87&gt;$C$11,B87&lt;=$C$12),1,0)*$D$12+IF(AND(B87&gt;$C$12,B87&lt;=$C$13),1,0)*$D$13+IF(AND(B87&gt;$C$13,B87&lt;=$C$14),1,0)*$D$14+IF(AND(B87&gt;$C$14,B87&lt;=$C$15),1,0)*$D$15+IF(AND(B87&gt;$C$15,B87&lt;=$C$16),1,0)*$D$16+IF(AND(B87&gt;$C$16,B87&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1456</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="G87" s="1">
         <v>16</v>
       </c>
-      <c r="H87" s="16">
+      <c r="H87" s="14">
         <f>ROUND(((F87-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,7 +2460,7 @@
         <f>($F$2*C88)+($H$2*D88)</f>
         <v>0</v>
       </c>
-      <c r="H88" s="16"/>
+      <c r="H88" s="14"/>
     </row>
     <row r="89" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -2498,14 +2471,14 @@
       </c>
       <c r="F89" s="1">
         <f>($E$88+B89)*(IF(B89&lt;=$C$8,1,0)*$D$8+IF(AND(B89&gt;$C$8,B89&lt;=$C$9),1,0)*$D$9+IF(AND(B89&gt;$C$9,B89&lt;=$C$10),1,0)*$D$10+IF(AND(B89&gt;$C$10,B89&lt;=$C$11),1,0)*$D$11+IF(AND(B89&gt;$C$11,B89&lt;=$C$12),1,0)*$D$12+IF(AND(B89&gt;$C$12,B89&lt;=$C$13),1,0)*$D$13+IF(AND(B89&gt;$C$13,B89&lt;=$C$14),1,0)*$D$14+IF(AND(B89&gt;$C$14,B89&lt;=$C$15),1,0)*$D$15+IF(AND(B89&gt;$C$15,B89&lt;=$C$16),1,0)*$D$16+IF(AND(B89&gt;$C$16,B89&lt;=$C$17),1,0)*$D$17)</f>
-        <v>532</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
       </c>
-      <c r="H89" s="16">
+      <c r="H89" s="14">
         <f>ROUND(((F89-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2517,14 +2490,14 @@
       </c>
       <c r="F90" s="1">
         <f>($E$88+B90)*(IF(B90&lt;=$C$8,1,0)*$D$8+IF(AND(B90&gt;$C$8,B90&lt;=$C$9),1,0)*$D$9+IF(AND(B90&gt;$C$9,B90&lt;=$C$10),1,0)*$D$10+IF(AND(B90&gt;$C$10,B90&lt;=$C$11),1,0)*$D$11+IF(AND(B90&gt;$C$11,B90&lt;=$C$12),1,0)*$D$12+IF(AND(B90&gt;$C$12,B90&lt;=$C$13),1,0)*$D$13+IF(AND(B90&gt;$C$13,B90&lt;=$C$14),1,0)*$D$14+IF(AND(B90&gt;$C$14,B90&lt;=$C$15),1,0)*$D$15+IF(AND(B90&gt;$C$15,B90&lt;=$C$16),1,0)*$D$16+IF(AND(B90&gt;$C$16,B90&lt;=$C$17),1,0)*$D$17)</f>
-        <v>860</v>
+        <v>4.3000000000000003E-2</v>
       </c>
       <c r="G90" s="1">
         <v>10</v>
       </c>
-      <c r="H90" s="16">
+      <c r="H90" s="14">
         <f>ROUND(((F90-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2536,14 +2509,14 @@
       </c>
       <c r="F91" s="1">
         <f>($E$88+B91)*(IF(B91&lt;=$C$8,1,0)*$D$8+IF(AND(B91&gt;$C$8,B91&lt;=$C$9),1,0)*$D$9+IF(AND(B91&gt;$C$9,B91&lt;=$C$10),1,0)*$D$10+IF(AND(B91&gt;$C$10,B91&lt;=$C$11),1,0)*$D$11+IF(AND(B91&gt;$C$11,B91&lt;=$C$12),1,0)*$D$12+IF(AND(B91&gt;$C$12,B91&lt;=$C$13),1,0)*$D$13+IF(AND(B91&gt;$C$13,B91&lt;=$C$14),1,0)*$D$14+IF(AND(B91&gt;$C$14,B91&lt;=$C$15),1,0)*$D$15+IF(AND(B91&gt;$C$15,B91&lt;=$C$16),1,0)*$D$16+IF(AND(B91&gt;$C$16,B91&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G91" s="1">
         <v>16</v>
       </c>
-      <c r="H91" s="16">
+      <c r="H91" s="14">
         <f>ROUND(((F91-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2561,7 +2534,7 @@
         <f>($F$2*C92)+($H$2*D92)</f>
         <v>0</v>
       </c>
-      <c r="H92" s="16"/>
+      <c r="H92" s="14"/>
     </row>
     <row r="93" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
@@ -2572,14 +2545,14 @@
       </c>
       <c r="F93" s="1">
         <f t="shared" ref="F93:F98" si="14">($E$92+B93)*(IF(B93&lt;=$C$8,1,0)*$D$8+IF(AND(B93&gt;$C$8,B93&lt;=$C$9),1,0)*$D$9+IF(AND(B93&gt;$C$9,B93&lt;=$C$10),1,0)*$D$10+IF(AND(B93&gt;$C$10,B93&lt;=$C$11),1,0)*$D$11+IF(AND(B93&gt;$C$11,B93&lt;=$C$12),1,0)*$D$12+IF(AND(B93&gt;$C$12,B93&lt;=$C$13),1,0)*$D$13+IF(AND(B93&gt;$C$13,B93&lt;=$C$14),1,0)*$D$14+IF(AND(B93&gt;$C$14,B93&lt;=$C$15),1,0)*$D$15+IF(AND(B93&gt;$C$15,B93&lt;=$C$16),1,0)*$D$16+IF(AND(B93&gt;$C$16,B93&lt;=$C$17),1,0)*$D$17)</f>
-        <v>532</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
       </c>
-      <c r="H93" s="16">
+      <c r="H93" s="14">
         <f t="shared" ref="H93:H98" si="15">ROUND(((F93-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2591,14 +2564,14 @@
       </c>
       <c r="F94" s="1">
         <f t="shared" si="14"/>
-        <v>860</v>
+        <v>4.3000000000000003E-2</v>
       </c>
       <c r="G94" s="1">
         <v>10</v>
       </c>
-      <c r="H94" s="16">
+      <c r="H94" s="14">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2610,14 +2583,14 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" si="14"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G95" s="1">
         <v>12</v>
       </c>
-      <c r="H95" s="16">
+      <c r="H95" s="14">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2629,14 +2602,14 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" si="14"/>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G96" s="1">
         <v>14</v>
       </c>
-      <c r="H96" s="16">
+      <c r="H96" s="14">
         <f t="shared" si="15"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2648,14 +2621,14 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" si="14"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G97" s="1">
         <v>16</v>
       </c>
-      <c r="H97" s="16">
+      <c r="H97" s="14">
         <f t="shared" si="15"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2667,14 +2640,14 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" si="14"/>
-        <v>1456</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="G98" s="1">
         <v>18</v>
       </c>
-      <c r="H98" s="16">
+      <c r="H98" s="14">
         <f t="shared" si="15"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -2692,7 +2665,7 @@
         <f>($F$2*C99)+($H$2*D99)</f>
         <v>0</v>
       </c>
-      <c r="H99" s="16"/>
+      <c r="H99" s="14"/>
     </row>
     <row r="100" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
@@ -2703,14 +2676,14 @@
       </c>
       <c r="F100" s="1">
         <f>($E$99+B100)*(IF(B100&lt;=$C$8,1,0)*$D$8+IF(AND(B100&gt;$C$8,B100&lt;=$C$9),1,0)*$D$9+IF(AND(B100&gt;$C$9,B100&lt;=$C$10),1,0)*$D$10+IF(AND(B100&gt;$C$10,B100&lt;=$C$11),1,0)*$D$11+IF(AND(B100&gt;$C$11,B100&lt;=$C$12),1,0)*$D$12+IF(AND(B100&gt;$C$12,B100&lt;=$C$13),1,0)*$D$13+IF(AND(B100&gt;$C$13,B100&lt;=$C$14),1,0)*$D$14+IF(AND(B100&gt;$C$14,B100&lt;=$C$15),1,0)*$D$15+IF(AND(B100&gt;$C$15,B100&lt;=$C$16),1,0)*$D$16+IF(AND(B100&gt;$C$16,B100&lt;=$C$17),1,0)*$D$17)</f>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>
       </c>
-      <c r="H100" s="16">
+      <c r="H100" s="14">
         <f t="shared" ref="H100:H111" si="16">ROUND(((F100-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2722,14 +2695,14 @@
       </c>
       <c r="F101" s="1">
         <f t="shared" ref="F101:F111" si="17">($E$99+B101)*(IF(B101&lt;=$C$8,1,0)*$D$8+IF(AND(B101&gt;$C$8,B101&lt;=$C$9),1,0)*$D$9+IF(AND(B101&gt;$C$9,B101&lt;=$C$10),1,0)*$D$10+IF(AND(B101&gt;$C$10,B101&lt;=$C$11),1,0)*$D$11+IF(AND(B101&gt;$C$11,B101&lt;=$C$12),1,0)*$D$12+IF(AND(B101&gt;$C$12,B101&lt;=$C$13),1,0)*$D$13+IF(AND(B101&gt;$C$13,B101&lt;=$C$14),1,0)*$D$14+IF(AND(B101&gt;$C$14,B101&lt;=$C$15),1,0)*$D$15+IF(AND(B101&gt;$C$15,B101&lt;=$C$16),1,0)*$D$16+IF(AND(B101&gt;$C$16,B101&lt;=$C$17),1,0)*$D$17)</f>
-        <v>532</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G101" s="1">
         <v>8</v>
       </c>
-      <c r="H101" s="16">
+      <c r="H101" s="14">
         <f t="shared" si="16"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2741,14 +2714,14 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" si="17"/>
-        <v>560</v>
+        <v>0.04</v>
       </c>
       <c r="G102" s="1">
         <v>8</v>
       </c>
-      <c r="H102" s="16">
+      <c r="H102" s="14">
         <f t="shared" si="16"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2760,14 +2733,14 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" si="17"/>
-        <v>672</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G103" s="1">
         <v>10</v>
       </c>
-      <c r="H103" s="16">
+      <c r="H103" s="14">
         <f t="shared" si="16"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2779,14 +2752,14 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" si="17"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G104" s="1">
         <v>12</v>
       </c>
-      <c r="H104" s="16">
+      <c r="H104" s="14">
         <f t="shared" si="16"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2798,14 +2771,14 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" si="17"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G105" s="1">
         <v>12</v>
       </c>
-      <c r="H105" s="16">
+      <c r="H105" s="14">
         <f t="shared" si="16"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2817,14 +2790,14 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" si="17"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G106" s="1">
         <v>14</v>
       </c>
-      <c r="H106" s="16">
+      <c r="H106" s="14">
         <f t="shared" si="16"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2836,14 +2809,14 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" si="17"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G107" s="1">
         <v>14</v>
       </c>
-      <c r="H107" s="16">
+      <c r="H107" s="14">
         <f t="shared" si="16"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2855,14 +2828,14 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" si="17"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G108" s="1">
         <v>16</v>
       </c>
-      <c r="H108" s="16">
+      <c r="H108" s="14">
         <f t="shared" si="16"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2874,14 +2847,14 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" si="17"/>
-        <v>1680</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="G109" s="1">
         <v>18</v>
       </c>
-      <c r="H109" s="16">
+      <c r="H109" s="14">
         <f t="shared" si="16"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2893,14 +2866,14 @@
       </c>
       <c r="F110" s="1">
         <f t="shared" si="17"/>
-        <v>1984</v>
+        <v>6.2E-2</v>
       </c>
       <c r="G110" s="1">
         <v>20</v>
       </c>
-      <c r="H110" s="16">
+      <c r="H110" s="14">
         <f t="shared" si="16"/>
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2912,14 +2885,14 @@
       </c>
       <c r="F111" s="1">
         <f t="shared" si="17"/>
-        <v>2336</v>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="G111" s="1">
         <v>25</v>
       </c>
-      <c r="H111" s="16">
+      <c r="H111" s="14">
         <f t="shared" si="16"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -2937,7 +2910,7 @@
         <f>($F$2*C112)+($H$2*D112)</f>
         <v>0</v>
       </c>
-      <c r="H112" s="16"/>
+      <c r="H112" s="14"/>
     </row>
     <row r="113" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
@@ -2948,14 +2921,14 @@
       </c>
       <c r="F113" s="1">
         <f>($E$112+B113)*(IF(B113&lt;=$C$8,1,0)*$D$8+IF(AND(B113&gt;$C$8,B113&lt;=$C$9),1,0)*$D$9+IF(AND(B113&gt;$C$9,B113&lt;=$C$10),1,0)*$D$10+IF(AND(B113&gt;$C$10,B113&lt;=$C$11),1,0)*$D$11+IF(AND(B113&gt;$C$11,B113&lt;=$C$12),1,0)*$D$12+IF(AND(B113&gt;$C$12,B113&lt;=$C$13),1,0)*$D$13+IF(AND(B113&gt;$C$13,B113&lt;=$C$14),1,0)*$D$14+IF(AND(B113&gt;$C$14,B113&lt;=$C$15),1,0)*$D$15+IF(AND(B113&gt;$C$15,B113&lt;=$C$16),1,0)*$D$16+IF(AND(B113&gt;$C$16,B113&lt;=$C$17),1,0)*$D$17)</f>
-        <v>518</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="G113" s="1">
         <v>0</v>
       </c>
-      <c r="H113" s="16">
+      <c r="H113" s="14">
         <f t="shared" ref="H113:H120" si="18">ROUND(((F113-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2967,14 +2940,14 @@
       </c>
       <c r="F114" s="1">
         <f t="shared" ref="F114:F120" si="19">($E$112+B114)*(IF(B114&lt;=$C$8,1,0)*$D$8+IF(AND(B114&gt;$C$8,B114&lt;=$C$9),1,0)*$D$9+IF(AND(B114&gt;$C$9,B114&lt;=$C$10),1,0)*$D$10+IF(AND(B114&gt;$C$10,B114&lt;=$C$11),1,0)*$D$11+IF(AND(B114&gt;$C$11,B114&lt;=$C$12),1,0)*$D$12+IF(AND(B114&gt;$C$12,B114&lt;=$C$13),1,0)*$D$13+IF(AND(B114&gt;$C$13,B114&lt;=$C$14),1,0)*$D$14+IF(AND(B114&gt;$C$14,B114&lt;=$C$15),1,0)*$D$15+IF(AND(B114&gt;$C$15,B114&lt;=$C$16),1,0)*$D$16+IF(AND(B114&gt;$C$16,B114&lt;=$C$17),1,0)*$D$17)</f>
-        <v>656</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G114" s="1">
         <v>6</v>
       </c>
-      <c r="H114" s="16">
+      <c r="H114" s="14">
         <f t="shared" si="18"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2986,14 +2959,14 @@
       </c>
       <c r="F115" s="1">
         <f t="shared" si="19"/>
-        <v>900</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="G115" s="1">
         <v>10</v>
       </c>
-      <c r="H115" s="16">
+      <c r="H115" s="14">
         <f t="shared" si="18"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3005,14 +2978,14 @@
       </c>
       <c r="F116" s="1">
         <f t="shared" si="19"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G116" s="1">
         <v>12</v>
       </c>
-      <c r="H116" s="16">
+      <c r="H116" s="14">
         <f t="shared" si="18"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3024,14 +2997,14 @@
       </c>
       <c r="F117" s="1">
         <f t="shared" si="19"/>
-        <v>1456</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="G117" s="1">
         <v>15</v>
       </c>
-      <c r="H117" s="16">
+      <c r="H117" s="14">
         <f t="shared" si="18"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3043,14 +3016,14 @@
       </c>
       <c r="F118" s="1">
         <f t="shared" si="19"/>
-        <v>1740</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G118" s="1">
         <v>18</v>
       </c>
-      <c r="H118" s="16">
+      <c r="H118" s="14">
         <f t="shared" si="18"/>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3062,14 +3035,14 @@
       </c>
       <c r="F119" s="1">
         <f t="shared" si="19"/>
-        <v>2080</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G119" s="1">
         <v>20</v>
       </c>
-      <c r="H119" s="16">
+      <c r="H119" s="14">
         <f t="shared" si="18"/>
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3081,14 +3054,14 @@
       </c>
       <c r="F120" s="1">
         <f t="shared" si="19"/>
-        <v>2336</v>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="G120" s="1">
         <v>25</v>
       </c>
-      <c r="H120" s="16">
+      <c r="H120" s="14">
         <f t="shared" si="18"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3106,7 +3079,7 @@
         <f>($F$2*C121)+($H$2*D121)</f>
         <v>0</v>
       </c>
-      <c r="H121" s="16"/>
+      <c r="H121" s="14"/>
     </row>
     <row r="122" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
@@ -3117,14 +3090,14 @@
       </c>
       <c r="F122" s="1">
         <f>($E$121+B122)*(IF(B122&lt;=$C$8,1,0)*$D$8+IF(AND(B122&gt;$C$8,B122&lt;=$C$9),1,0)*$D$9+IF(AND(B122&gt;$C$9,B122&lt;=$C$10),1,0)*$D$10+IF(AND(B122&gt;$C$10,B122&lt;=$C$11),1,0)*$D$11+IF(AND(B122&gt;$C$11,B122&lt;=$C$12),1,0)*$D$12+IF(AND(B122&gt;$C$12,B122&lt;=$C$13),1,0)*$D$13+IF(AND(B122&gt;$C$13,B122&lt;=$C$14),1,0)*$D$14+IF(AND(B122&gt;$C$14,B122&lt;=$C$15),1,0)*$D$15+IF(AND(B122&gt;$C$15,B122&lt;=$C$16),1,0)*$D$16+IF(AND(B122&gt;$C$16,B122&lt;=$C$17),1,0)*$D$17)</f>
-        <v>518</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="G122" s="1">
         <v>0</v>
       </c>
-      <c r="H122" s="16">
+      <c r="H122" s="14">
         <f t="shared" ref="H122:H129" si="20">ROUND(((F122-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3136,14 +3109,14 @@
       </c>
       <c r="F123" s="1">
         <f t="shared" ref="F123:F129" si="21">($E$121+B123)*(IF(B123&lt;=$C$8,1,0)*$D$8+IF(AND(B123&gt;$C$8,B123&lt;=$C$9),1,0)*$D$9+IF(AND(B123&gt;$C$9,B123&lt;=$C$10),1,0)*$D$10+IF(AND(B123&gt;$C$10,B123&lt;=$C$11),1,0)*$D$11+IF(AND(B123&gt;$C$11,B123&lt;=$C$12),1,0)*$D$12+IF(AND(B123&gt;$C$12,B123&lt;=$C$13),1,0)*$D$13+IF(AND(B123&gt;$C$13,B123&lt;=$C$14),1,0)*$D$14+IF(AND(B123&gt;$C$14,B123&lt;=$C$15),1,0)*$D$15+IF(AND(B123&gt;$C$15,B123&lt;=$C$16),1,0)*$D$16+IF(AND(B123&gt;$C$16,B123&lt;=$C$17),1,0)*$D$17)</f>
-        <v>656</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G123" s="1">
         <v>6</v>
       </c>
-      <c r="H123" s="16">
+      <c r="H123" s="14">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3155,14 +3128,14 @@
       </c>
       <c r="F124" s="1">
         <f t="shared" si="21"/>
-        <v>900</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="G124" s="1">
         <v>10</v>
       </c>
-      <c r="H124" s="16">
+      <c r="H124" s="14">
         <f t="shared" si="20"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3174,14 +3147,14 @@
       </c>
       <c r="F125" s="1">
         <f t="shared" si="21"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G125" s="1">
         <v>12</v>
       </c>
-      <c r="H125" s="16">
+      <c r="H125" s="14">
         <f t="shared" si="20"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3193,14 +3166,14 @@
       </c>
       <c r="F126" s="1">
         <f t="shared" si="21"/>
-        <v>1456</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="G126" s="1">
         <v>15</v>
       </c>
-      <c r="H126" s="16">
+      <c r="H126" s="14">
         <f t="shared" si="20"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3212,14 +3185,14 @@
       </c>
       <c r="F127" s="1">
         <f t="shared" si="21"/>
-        <v>1740</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G127" s="1">
         <v>18</v>
       </c>
-      <c r="H127" s="16">
+      <c r="H127" s="14">
         <f t="shared" si="20"/>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3231,14 +3204,14 @@
       </c>
       <c r="F128" s="1">
         <f t="shared" si="21"/>
-        <v>2080</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G128" s="1">
         <v>20</v>
       </c>
-      <c r="H128" s="16">
+      <c r="H128" s="14">
         <f t="shared" si="20"/>
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3250,14 +3223,14 @@
       </c>
       <c r="F129" s="1">
         <f t="shared" si="21"/>
-        <v>2336</v>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="G129" s="1">
         <v>25</v>
       </c>
-      <c r="H129" s="16">
+      <c r="H129" s="14">
         <f t="shared" si="20"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3275,7 +3248,7 @@
         <f>($F$2*C130)+($H$2*D130)</f>
         <v>0</v>
       </c>
-      <c r="H130" s="16"/>
+      <c r="H130" s="14"/>
     </row>
     <row r="131" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
@@ -3286,14 +3259,14 @@
       </c>
       <c r="F131" s="1">
         <f>($E$130+B131)*(IF(B131&lt;=$C$8,1,0)*$D$8+IF(AND(B131&gt;$C$8,B131&lt;=$C$9),1,0)*$D$9+IF(AND(B131&gt;$C$9,B131&lt;=$C$10),1,0)*$D$10+IF(AND(B131&gt;$C$10,B131&lt;=$C$11),1,0)*$D$11+IF(AND(B131&gt;$C$11,B131&lt;=$C$12),1,0)*$D$12+IF(AND(B131&gt;$C$12,B131&lt;=$C$13),1,0)*$D$13+IF(AND(B131&gt;$C$13,B131&lt;=$C$14),1,0)*$D$14+IF(AND(B131&gt;$C$14,B131&lt;=$C$15),1,0)*$D$15+IF(AND(B131&gt;$C$15,B131&lt;=$C$16),1,0)*$D$16+IF(AND(B131&gt;$C$16,B131&lt;=$C$17),1,0)*$D$17)</f>
-        <v>432</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
       </c>
-      <c r="H131" s="16">
+      <c r="H131" s="14">
         <f t="shared" ref="H131:H149" si="22">ROUND(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3305,14 +3278,14 @@
       </c>
       <c r="F132" s="1">
         <f t="shared" ref="F132:F149" si="23">($E$130+B132)*(IF(B132&lt;=$C$8,1,0)*$D$8+IF(AND(B132&gt;$C$8,B132&lt;=$C$9),1,0)*$D$9+IF(AND(B132&gt;$C$9,B132&lt;=$C$10),1,0)*$D$10+IF(AND(B132&gt;$C$10,B132&lt;=$C$11),1,0)*$D$11+IF(AND(B132&gt;$C$11,B132&lt;=$C$12),1,0)*$D$12+IF(AND(B132&gt;$C$12,B132&lt;=$C$13),1,0)*$D$13+IF(AND(B132&gt;$C$13,B132&lt;=$C$14),1,0)*$D$14+IF(AND(B132&gt;$C$14,B132&lt;=$C$15),1,0)*$D$15+IF(AND(B132&gt;$C$15,B132&lt;=$C$16),1,0)*$D$16+IF(AND(B132&gt;$C$16,B132&lt;=$C$17),1,0)*$D$17)</f>
-        <v>518</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="G132" s="1">
         <v>3</v>
       </c>
-      <c r="H132" s="16">
+      <c r="H132" s="14">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3324,14 +3297,14 @@
       </c>
       <c r="F133" s="1">
         <f t="shared" si="23"/>
-        <v>532</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
       </c>
-      <c r="H133" s="16">
+      <c r="H133" s="14">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3343,14 +3316,14 @@
       </c>
       <c r="F134" s="1">
         <f t="shared" si="23"/>
-        <v>560</v>
+        <v>0.04</v>
       </c>
       <c r="G134" s="1">
         <v>8</v>
       </c>
-      <c r="H134" s="16">
+      <c r="H134" s="14">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3362,14 +3335,14 @@
       </c>
       <c r="F135" s="1">
         <f t="shared" si="23"/>
-        <v>656</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G135" s="1">
         <v>12</v>
       </c>
-      <c r="H135" s="16">
+      <c r="H135" s="14">
         <f t="shared" si="22"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3381,14 +3354,14 @@
       </c>
       <c r="F136" s="1">
         <f t="shared" si="23"/>
-        <v>672</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G136" s="1">
         <v>10</v>
       </c>
-      <c r="H136" s="16">
+      <c r="H136" s="14">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3400,14 +3373,14 @@
       </c>
       <c r="F137" s="1">
         <f t="shared" si="23"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G137" s="1">
         <v>12</v>
       </c>
-      <c r="H137" s="16">
+      <c r="H137" s="14">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3419,14 +3392,14 @@
       </c>
       <c r="F138" s="1">
         <f t="shared" si="23"/>
-        <v>880</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="G138" s="1">
         <v>12</v>
       </c>
-      <c r="H138" s="16">
+      <c r="H138" s="14">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3438,14 +3411,14 @@
       </c>
       <c r="F139" s="1">
         <f t="shared" si="23"/>
-        <v>900</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="G139" s="1">
         <v>14</v>
       </c>
-      <c r="H139" s="16">
+      <c r="H139" s="14">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3457,14 +3430,14 @@
       </c>
       <c r="F140" s="1">
         <f t="shared" si="23"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G140" s="1">
         <v>14</v>
       </c>
-      <c r="H140" s="16">
+      <c r="H140" s="14">
         <f t="shared" si="22"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3476,14 +3449,14 @@
       </c>
       <c r="F141" s="1">
         <f t="shared" si="23"/>
-        <v>1248</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G141" s="1">
         <v>14</v>
       </c>
-      <c r="H141" s="16">
+      <c r="H141" s="14">
         <f t="shared" si="22"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3495,14 +3468,14 @@
       </c>
       <c r="F142" s="1">
         <f t="shared" si="23"/>
-        <v>1274</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="G142" s="1">
         <v>15</v>
       </c>
-      <c r="H142" s="16">
+      <c r="H142" s="14">
         <f t="shared" si="22"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3514,14 +3487,14 @@
       </c>
       <c r="F143" s="1">
         <f t="shared" si="23"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G143" s="1">
         <v>16</v>
       </c>
-      <c r="H143" s="16">
+      <c r="H143" s="14">
         <f t="shared" si="22"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3533,14 +3506,14 @@
       </c>
       <c r="F144" s="1">
         <f t="shared" si="23"/>
-        <v>1456</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="G144" s="1">
         <v>17</v>
       </c>
-      <c r="H144" s="16">
+      <c r="H144" s="14">
         <f t="shared" si="22"/>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3552,14 +3525,14 @@
       </c>
       <c r="F145" s="1">
         <f t="shared" si="23"/>
-        <v>1680</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="G145" s="1">
         <v>18</v>
       </c>
-      <c r="H145" s="16">
+      <c r="H145" s="14">
         <f t="shared" si="22"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3571,14 +3544,14 @@
       </c>
       <c r="F146" s="1">
         <f t="shared" si="23"/>
-        <v>1740</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G146" s="1">
         <v>18</v>
       </c>
-      <c r="H146" s="16">
+      <c r="H146" s="14">
         <f t="shared" si="22"/>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3590,14 +3563,14 @@
       </c>
       <c r="F147" s="1">
         <f t="shared" si="23"/>
-        <v>1984</v>
+        <v>6.2E-2</v>
       </c>
       <c r="G147" s="1">
         <v>20</v>
       </c>
-      <c r="H147" s="16">
+      <c r="H147" s="14">
         <f t="shared" si="22"/>
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3609,14 +3582,14 @@
       </c>
       <c r="F148" s="1">
         <f t="shared" si="23"/>
-        <v>2336</v>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="G148" s="1">
         <v>24</v>
       </c>
-      <c r="H148" s="16">
+      <c r="H148" s="14">
         <f t="shared" si="22"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3628,14 +3601,14 @@
       </c>
       <c r="F149" s="1">
         <f t="shared" si="23"/>
-        <v>2336</v>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="G149" s="1">
         <v>25</v>
       </c>
-      <c r="H149" s="16">
+      <c r="H149" s="14">
         <f t="shared" si="22"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -3653,7 +3626,7 @@
         <f>($F$2*C150)+($H$2*D150)</f>
         <v>0</v>
       </c>
-      <c r="H150" s="16"/>
+      <c r="H150" s="14"/>
     </row>
     <row r="151" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
@@ -3664,14 +3637,14 @@
       </c>
       <c r="F151" s="1">
         <f>($E$150+B151)*(IF(B151&lt;=$C$8,1,0)*$D$8+IF(AND(B151&gt;$C$8,B151&lt;=$C$9),1,0)*$D$9+IF(AND(B151&gt;$C$9,B151&lt;=$C$10),1,0)*$D$10+IF(AND(B151&gt;$C$10,B151&lt;=$C$11),1,0)*$D$11+IF(AND(B151&gt;$C$11,B151&lt;=$C$12),1,0)*$D$12+IF(AND(B151&gt;$C$12,B151&lt;=$C$13),1,0)*$D$13+IF(AND(B151&gt;$C$13,B151&lt;=$C$14),1,0)*$D$14+IF(AND(B151&gt;$C$14,B151&lt;=$C$15),1,0)*$D$15+IF(AND(B151&gt;$C$15,B151&lt;=$C$16),1,0)*$D$16+IF(AND(B151&gt;$C$16,B151&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1512</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G151" s="1">
         <v>0</v>
       </c>
-      <c r="H151" s="16">
+      <c r="H151" s="14">
         <f>ROUND(((F151-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3683,14 +3656,14 @@
       </c>
       <c r="F152" s="1">
         <f>($E$150+B152)*(IF(B152&lt;=$C$8,1,0)*$D$8+IF(AND(B152&gt;$C$8,B152&lt;=$C$9),1,0)*$D$9+IF(AND(B152&gt;$C$9,B152&lt;=$C$10),1,0)*$D$10+IF(AND(B152&gt;$C$10,B152&lt;=$C$11),1,0)*$D$11+IF(AND(B152&gt;$C$11,B152&lt;=$C$12),1,0)*$D$12+IF(AND(B152&gt;$C$12,B152&lt;=$C$13),1,0)*$D$13+IF(AND(B152&gt;$C$13,B152&lt;=$C$14),1,0)*$D$14+IF(AND(B152&gt;$C$14,B152&lt;=$C$15),1,0)*$D$15+IF(AND(B152&gt;$C$15,B152&lt;=$C$16),1,0)*$D$16+IF(AND(B152&gt;$C$16,B152&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1800</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="G152" s="1">
         <v>6</v>
       </c>
-      <c r="H152" s="16">
+      <c r="H152" s="14">
         <f>ROUND(((F152-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3702,14 +3675,14 @@
       </c>
       <c r="F153" s="1">
         <f>($E$150+B153)*(IF(B153&lt;=$C$8,1,0)*$D$8+IF(AND(B153&gt;$C$8,B153&lt;=$C$9),1,0)*$D$9+IF(AND(B153&gt;$C$9,B153&lt;=$C$10),1,0)*$D$10+IF(AND(B153&gt;$C$10,B153&lt;=$C$11),1,0)*$D$11+IF(AND(B153&gt;$C$11,B153&lt;=$C$12),1,0)*$D$12+IF(AND(B153&gt;$C$12,B153&lt;=$C$13),1,0)*$D$13+IF(AND(B153&gt;$C$13,B153&lt;=$C$14),1,0)*$D$14+IF(AND(B153&gt;$C$14,B153&lt;=$C$15),1,0)*$D$15+IF(AND(B153&gt;$C$15,B153&lt;=$C$16),1,0)*$D$16+IF(AND(B153&gt;$C$16,B153&lt;=$C$17),1,0)*$D$17)</f>
-        <v>2240</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G153" s="1">
         <v>10</v>
       </c>
-      <c r="H153" s="16">
+      <c r="H153" s="14">
         <f>ROUND(((F153-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3721,14 +3694,14 @@
       </c>
       <c r="F154" s="1">
         <f>($E$150+B154)*(IF(B154&lt;=$C$8,1,0)*$D$8+IF(AND(B154&gt;$C$8,B154&lt;=$C$9),1,0)*$D$9+IF(AND(B154&gt;$C$9,B154&lt;=$C$10),1,0)*$D$10+IF(AND(B154&gt;$C$10,B154&lt;=$C$11),1,0)*$D$11+IF(AND(B154&gt;$C$11,B154&lt;=$C$12),1,0)*$D$12+IF(AND(B154&gt;$C$12,B154&lt;=$C$13),1,0)*$D$13+IF(AND(B154&gt;$C$13,B154&lt;=$C$14),1,0)*$D$14+IF(AND(B154&gt;$C$14,B154&lt;=$C$15),1,0)*$D$15+IF(AND(B154&gt;$C$15,B154&lt;=$C$16),1,0)*$D$16+IF(AND(B154&gt;$C$16,B154&lt;=$C$17),1,0)*$D$17)</f>
-        <v>2400</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G154" s="1">
         <v>16</v>
       </c>
-      <c r="H154" s="16">
+      <c r="H154" s="14">
         <f>ROUND(((F154-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -3746,7 +3719,7 @@
         <f>($F$2*C155)+($H$2*D155)</f>
         <v>0</v>
       </c>
-      <c r="H155" s="16"/>
+      <c r="H155" s="14"/>
     </row>
     <row r="156" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
@@ -3757,14 +3730,14 @@
       </c>
       <c r="F156" s="1">
         <f>($E$155+B156)*(IF(B156&lt;=$C$8,1,0)*$D$8+IF(AND(B156&gt;$C$8,B156&lt;=$C$9),1,0)*$D$9+IF(AND(B156&gt;$C$9,B156&lt;=$C$10),1,0)*$D$10+IF(AND(B156&gt;$C$10,B156&lt;=$C$11),1,0)*$D$11+IF(AND(B156&gt;$C$11,B156&lt;=$C$12),1,0)*$D$12+IF(AND(B156&gt;$C$12,B156&lt;=$C$13),1,0)*$D$13+IF(AND(B156&gt;$C$13,B156&lt;=$C$14),1,0)*$D$14+IF(AND(B156&gt;$C$14,B156&lt;=$C$15),1,0)*$D$15+IF(AND(B156&gt;$C$15,B156&lt;=$C$16),1,0)*$D$16+IF(AND(B156&gt;$C$16,B156&lt;=$C$17),1,0)*$D$17)</f>
-        <v>672</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G156" s="1">
         <v>0</v>
       </c>
-      <c r="H156" s="16">
+      <c r="H156" s="14">
         <f t="shared" ref="H156:H164" si="24">ROUND(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3776,14 +3749,14 @@
       </c>
       <c r="F157" s="1">
         <f t="shared" ref="F157:F164" si="25">($E$155+B157)*(IF(B157&lt;=$C$8,1,0)*$D$8+IF(AND(B157&gt;$C$8,B157&lt;=$C$9),1,0)*$D$9+IF(AND(B157&gt;$C$9,B157&lt;=$C$10),1,0)*$D$10+IF(AND(B157&gt;$C$10,B157&lt;=$C$11),1,0)*$D$11+IF(AND(B157&gt;$C$11,B157&lt;=$C$12),1,0)*$D$12+IF(AND(B157&gt;$C$12,B157&lt;=$C$13),1,0)*$D$13+IF(AND(B157&gt;$C$13,B157&lt;=$C$14),1,0)*$D$14+IF(AND(B157&gt;$C$14,B157&lt;=$C$15),1,0)*$D$15+IF(AND(B157&gt;$C$15,B157&lt;=$C$16),1,0)*$D$16+IF(AND(B157&gt;$C$16,B157&lt;=$C$17),1,0)*$D$17)</f>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G157" s="1">
         <v>0</v>
       </c>
-      <c r="H157" s="16">
+      <c r="H157" s="14">
         <f t="shared" si="24"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3795,14 +3768,14 @@
       </c>
       <c r="F158" s="1">
         <f t="shared" si="25"/>
-        <v>1104</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G158" s="1">
         <v>2</v>
       </c>
-      <c r="H158" s="16">
+      <c r="H158" s="14">
         <f t="shared" si="24"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3814,14 +3787,14 @@
       </c>
       <c r="F159" s="1">
         <f t="shared" si="25"/>
-        <v>1300</v>
+        <v>0.05</v>
       </c>
       <c r="G159" s="1">
         <v>6</v>
       </c>
-      <c r="H159" s="16">
+      <c r="H159" s="14">
         <f t="shared" si="24"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3833,14 +3806,14 @@
       </c>
       <c r="F160" s="1">
         <f t="shared" si="25"/>
-        <v>1512</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G160" s="1">
         <v>6</v>
       </c>
-      <c r="H160" s="16">
+      <c r="H160" s="14">
         <f t="shared" si="24"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3852,14 +3825,14 @@
       </c>
       <c r="F161" s="1">
         <f t="shared" si="25"/>
-        <v>1512</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G161" s="1">
         <v>11</v>
       </c>
-      <c r="H161" s="16">
+      <c r="H161" s="14">
         <f t="shared" si="24"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3871,14 +3844,14 @@
       </c>
       <c r="F162" s="1">
         <f t="shared" si="25"/>
-        <v>1800</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="G162" s="1">
         <v>10</v>
       </c>
-      <c r="H162" s="16">
+      <c r="H162" s="14">
         <f t="shared" si="24"/>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3890,14 +3863,14 @@
       </c>
       <c r="F163" s="1">
         <f t="shared" si="25"/>
-        <v>2240</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G163" s="1">
         <v>16</v>
       </c>
-      <c r="H163" s="16">
+      <c r="H163" s="14">
         <f t="shared" si="24"/>
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3909,14 +3882,14 @@
       </c>
       <c r="F164" s="1">
         <f t="shared" si="25"/>
-        <v>2400</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G164" s="1">
         <v>16</v>
       </c>
-      <c r="H164" s="16">
+      <c r="H164" s="14">
         <f t="shared" si="24"/>
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>